<commit_message>
update the units file 23 shahrivar
</commit_message>
<xml_diff>
--- a/PythonScripts/units.xlsx
+++ b/PythonScripts/units.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\TelegramBot\TelegramBot\TelegramBot\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8CDADC-B5F9-4F38-AE48-3EF594C016F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4481C51D-875F-4DAC-836F-309DA8EC18CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
   <si>
     <t>طبقه</t>
   </si>
@@ -89,14 +89,21 @@
   <si>
     <t>پریمیوم   B</t>
   </si>
+  <si>
+    <t xml:space="preserve">جاده اصلی  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> غروب خورشید  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_([$AED]\ * #,##0_);_([$AED]\ * \(#,##0\);_([$AED]\ * &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$AED]\ * #,##0_);_([$AED]\ * \(#,##0\);_([$AED]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$AED]\ * #,##0.00_);_([$AED]\ * \(#,##0.00\);_([$AED]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -217,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -283,6 +290,18 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,10 +619,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -686,22 +705,22 @@
         <v>14</v>
       </c>
       <c r="H2" s="18">
-        <f t="shared" ref="H2:H53" si="0">I2/F2</f>
+        <f t="shared" ref="H2:H62" si="0">I2/F2</f>
         <v>22783.785321165396</v>
       </c>
       <c r="I2" s="19">
-        <f>(K2*100)/85</f>
+        <f t="shared" ref="I2:I9" si="1">(K2*100)/85</f>
         <v>1014783.4235294118</v>
       </c>
       <c r="J2" s="18">
-        <f t="shared" ref="J2:J53" si="1">K2/F2</f>
+        <f t="shared" ref="J2:J62" si="2">K2/F2</f>
         <v>19366.217522990588</v>
       </c>
       <c r="K2" s="19">
         <v>862565.91</v>
       </c>
       <c r="L2" s="18">
-        <f t="shared" ref="L2:L53" si="2">M2/F2</f>
+        <f t="shared" ref="L2:L62" si="3">M2/F2</f>
         <v>18227.028283346281</v>
       </c>
       <c r="M2" s="19">
@@ -735,18 +754,18 @@
         <v>23083.458260440148</v>
       </c>
       <c r="I3" s="19">
-        <f t="shared" ref="I3:I56" si="3">(K3*100)/85</f>
+        <f t="shared" si="1"/>
         <v>1028135.8352941177</v>
       </c>
       <c r="J3" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19620.939521374123</v>
       </c>
       <c r="K3" s="19">
         <v>873915.46</v>
       </c>
       <c r="L3" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18466.766647972869</v>
       </c>
       <c r="M3" s="19">
@@ -780,18 +799,18 @@
         <v>17702.334827701921</v>
       </c>
       <c r="I4" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1284478.2</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15046.984603546634</v>
       </c>
       <c r="K4" s="20">
         <v>1091806.47</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14161.867862161538</v>
       </c>
       <c r="M4" s="20">
@@ -825,18 +844,18 @@
         <v>17762.358196522</v>
       </c>
       <c r="I5" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1289361.5411764707</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15098.0044670437</v>
       </c>
       <c r="K5" s="20">
         <v>1095957.31</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14209.886516699693</v>
       </c>
       <c r="M5" s="20">
@@ -870,18 +889,18 @@
         <v>17237.713883579599</v>
       </c>
       <c r="I6" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1314024.0823529412</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14652.05680104266</v>
       </c>
       <c r="K6" s="20">
         <v>1116920.47</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13790.171160880058</v>
       </c>
       <c r="M6" s="20">
@@ -915,18 +934,18 @@
         <v>17237.533054557545</v>
       </c>
       <c r="I7" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1334364.4823529411</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14651.903096373917</v>
       </c>
       <c r="K7" s="20">
         <v>1134209.81</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13790.026367656867</v>
       </c>
       <c r="M7" s="20">
@@ -960,18 +979,18 @@
         <v>17327.467912358661</v>
       </c>
       <c r="I8" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1341326.3764705881</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14728.347725504864</v>
       </c>
       <c r="K8" s="20">
         <v>1140127.42</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13861.974443870691</v>
       </c>
       <c r="M8" s="20">
@@ -1005,18 +1024,18 @@
         <v>17567.283272292621</v>
       </c>
       <c r="I9" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1345310.5176470589</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14932.190781448728</v>
       </c>
       <c r="K9" s="20">
         <v>1143513.94</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14053.826694646816</v>
       </c>
       <c r="M9" s="20">
@@ -1028,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -1036,134 +1055,133 @@
       <c r="D10" s="6">
         <v>65.150000000000006</v>
       </c>
-      <c r="E10" s="7">
-        <v>13.950314479999999</v>
-      </c>
-      <c r="F10" s="7">
-        <v>79.100314480000009</v>
+      <c r="E10" s="6">
+        <v>12.26</v>
+      </c>
+      <c r="F10" s="6">
+        <v>77.410000000000011</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>17387.447344332941</v>
-      </c>
-      <c r="I10" s="20">
-        <f t="shared" si="3"/>
-        <v>1375352.5529411766</v>
+        <v>17387.516432745426</v>
+      </c>
+      <c r="I10" s="22">
+        <v>1345967.6470588236</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="1"/>
-        <v>14779.330242682998</v>
+        <f t="shared" si="2"/>
+        <v>14779.388967833611</v>
       </c>
       <c r="K10" s="20">
-        <v>1169049.67</v>
+        <v>1144072.5</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" si="2"/>
-        <v>13909.957845720059</v>
-      </c>
-      <c r="M10" s="20">
-        <v>1100282.04</v>
+        <f t="shared" si="3"/>
+        <v>13910.013176592171</v>
+      </c>
+      <c r="M10" s="23">
+        <v>1076774.1200000001</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="6">
-        <v>617</v>
+        <v>423</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="6">
-        <v>66.69</v>
+        <v>65.150000000000006</v>
       </c>
       <c r="E11" s="7">
-        <v>11.689984490000001</v>
+        <v>13.950314479999999</v>
       </c>
       <c r="F11" s="7">
-        <v>78.379984489999998</v>
+        <v>79.100314480000009</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>17567.390865012047</v>
+        <v>17387.447344332941</v>
       </c>
       <c r="I11" s="20">
-        <f t="shared" si="3"/>
-        <v>1376931.8235294118</v>
+        <f t="shared" ref="I11:I23" si="4">(K11*100)/85</f>
+        <v>1375352.5529411766</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="1"/>
-        <v>14932.28223526024</v>
+        <f t="shared" si="2"/>
+        <v>14779.330242682998</v>
       </c>
       <c r="K11" s="20">
-        <v>1170392.05</v>
+        <v>1169049.67</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="2"/>
-        <v>14053.912579435877</v>
+        <f t="shared" si="3"/>
+        <v>13909.957845720059</v>
       </c>
       <c r="M11" s="20">
-        <v>1101545.45</v>
+        <v>1100282.04</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" s="6">
-        <v>312</v>
+        <v>617</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="6">
-        <v>66.67</v>
+        <v>66.69</v>
       </c>
       <c r="E12" s="7">
-        <v>14.93973143</v>
+        <v>11.689984490000001</v>
       </c>
       <c r="F12" s="7">
-        <v>81.609731429999997</v>
+        <v>78.379984489999998</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>17237.680865167295</v>
+        <v>17567.390865012047</v>
       </c>
       <c r="I12" s="20">
-        <f t="shared" si="3"/>
-        <v>1406762.5058823528</v>
+        <f t="shared" si="4"/>
+        <v>1376931.8235294118</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="1"/>
-        <v>14652.028735392199</v>
+        <f t="shared" si="2"/>
+        <v>14932.28223526024</v>
       </c>
       <c r="K12" s="20">
-        <v>1195748.1299999999</v>
+        <v>1170392.05</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.144634470586</v>
+        <f t="shared" si="3"/>
+        <v>14053.912579435877</v>
       </c>
       <c r="M12" s="20">
-        <v>1125410</v>
+        <v>1101545.45</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" s="6">
-        <v>612</v>
+        <v>312</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -1172,125 +1190,125 @@
         <v>66.67</v>
       </c>
       <c r="E13" s="7">
-        <v>13.58985084</v>
+        <v>14.93973143</v>
       </c>
       <c r="F13" s="7">
-        <v>80.259850839999999</v>
+        <v>81.609731429999997</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="0"/>
-        <v>17567.419963103846</v>
+        <v>17237.680865167295</v>
       </c>
       <c r="I13" s="20">
-        <f t="shared" si="3"/>
-        <v>1409958.5058823531</v>
+        <f t="shared" si="4"/>
+        <v>1406762.5058823528</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="1"/>
-        <v>14932.306968638268</v>
+        <f t="shared" si="2"/>
+        <v>14652.028735392199</v>
       </c>
       <c r="K13" s="20">
-        <v>1198464.73</v>
+        <v>1195748.1299999999</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="2"/>
-        <v>14053.936036445293</v>
+        <f t="shared" si="3"/>
+        <v>13790.144634470586</v>
       </c>
       <c r="M13" s="20">
-        <v>1127966.81</v>
+        <v>1125410</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B14" s="6">
-        <v>230</v>
+        <v>612</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
       </c>
       <c r="D14" s="6">
-        <v>68.77</v>
+        <v>66.67</v>
       </c>
       <c r="E14" s="7">
-        <v>14.33028775</v>
+        <v>13.58985084</v>
       </c>
       <c r="F14" s="7">
-        <v>83.100287749999993</v>
+        <v>80.259850839999999</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="0"/>
-        <v>17237.564435580218</v>
+        <v>17567.419963103846</v>
       </c>
       <c r="I14" s="20">
-        <f t="shared" si="3"/>
-        <v>1432446.5647058825</v>
+        <f t="shared" si="4"/>
+        <v>1409958.5058823531</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="1"/>
-        <v>14651.929770243187</v>
+        <f t="shared" si="2"/>
+        <v>14932.306968638268</v>
       </c>
       <c r="K14" s="20">
-        <v>1217579.58</v>
+        <v>1198464.73</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.051527228317</v>
+        <f t="shared" si="3"/>
+        <v>14053.936036445293</v>
       </c>
       <c r="M14" s="20">
-        <v>1145957.25</v>
+        <v>1127966.81</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="6">
-        <v>114</v>
+        <v>230</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15" s="6">
-        <v>65.150000000000006</v>
+        <v>68.77</v>
       </c>
       <c r="E15" s="7">
-        <v>18.26008465</v>
+        <v>14.33028775</v>
       </c>
       <c r="F15" s="7">
-        <v>83.410084650000002</v>
+        <v>83.100287749999993</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="0"/>
-        <v>17237.606574343787</v>
+        <v>17237.564435580218</v>
       </c>
       <c r="I15" s="20">
-        <f t="shared" si="3"/>
-        <v>1437790.2235294117</v>
+        <f t="shared" si="4"/>
+        <v>1432446.5647058825</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="1"/>
-        <v>14651.965588192217</v>
+        <f t="shared" si="2"/>
+        <v>14651.929770243187</v>
       </c>
       <c r="K15" s="20">
-        <v>1222121.69</v>
+        <v>1217579.58</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.085273579685</v>
+        <f t="shared" si="3"/>
+        <v>13790.051527228317</v>
       </c>
       <c r="M15" s="20">
-        <v>1150232.18</v>
+        <v>1145957.25</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1298,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="6">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -1320,18 +1338,18 @@
         <v>17237.606574343787</v>
       </c>
       <c r="I16" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1437790.2235294117</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14651.965588192217</v>
       </c>
       <c r="K16" s="20">
         <v>1222121.69</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13790.085273579685</v>
       </c>
       <c r="M16" s="20">
@@ -1340,92 +1358,92 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B17" s="6">
-        <v>430</v>
+        <v>125</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="6">
-        <v>68.77</v>
+        <v>65.150000000000006</v>
       </c>
       <c r="E17" s="7">
-        <v>14.33028775</v>
+        <v>18.26008465</v>
       </c>
       <c r="F17" s="7">
-        <v>83.100287749999993</v>
+        <v>83.410084650000002</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>17327.499566931405</v>
+        <v>17237.606574343787</v>
       </c>
       <c r="I17" s="20">
-        <f t="shared" si="3"/>
-        <v>1439920.2</v>
+        <f t="shared" si="4"/>
+        <v>1437790.2235294117</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="1"/>
-        <v>14728.374631891693</v>
+        <f t="shared" si="2"/>
+        <v>14651.965588192217</v>
       </c>
       <c r="K17" s="20">
-        <v>1223932.17</v>
+        <v>1222121.69</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="2"/>
-        <v>13861.999653545123</v>
+        <f t="shared" si="3"/>
+        <v>13790.085273579685</v>
       </c>
       <c r="M17" s="20">
-        <v>1151936.1599999999</v>
+        <v>1150232.18</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B18" s="6">
-        <v>216</v>
+        <v>430</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="6">
-        <v>65.150000000000006</v>
+        <v>68.77</v>
       </c>
       <c r="E18" s="7">
-        <v>18.629838589999999</v>
+        <v>14.33028775</v>
       </c>
       <c r="F18" s="7">
-        <v>83.779838589999997</v>
+        <v>83.100287749999993</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>17237.657239278175</v>
+        <v>17327.499566931405</v>
       </c>
       <c r="I18" s="20">
-        <f t="shared" si="3"/>
-        <v>1444168.1411764706</v>
+        <f t="shared" si="4"/>
+        <v>1439920.2</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="1"/>
-        <v>14652.008653386449</v>
+        <f t="shared" si="2"/>
+        <v>14728.374631891693</v>
       </c>
       <c r="K18" s="20">
-        <v>1227542.92</v>
+        <v>1223932.17</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.125875676984</v>
+        <f t="shared" si="3"/>
+        <v>13861.999653545123</v>
       </c>
       <c r="M18" s="20">
-        <v>1155334.52</v>
+        <v>1151936.1599999999</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1433,187 +1451,187 @@
         <v>2</v>
       </c>
       <c r="B19" s="6">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
       <c r="D19" s="6">
-        <v>66.69</v>
+        <v>65.150000000000006</v>
       </c>
       <c r="E19" s="7">
-        <v>17.760266509999997</v>
+        <v>18.629838589999999</v>
       </c>
       <c r="F19" s="7">
-        <v>84.450266509999992</v>
+        <v>83.779838589999997</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>17237.569673848226</v>
+        <v>17237.657239278175</v>
       </c>
       <c r="I19" s="20">
-        <f t="shared" si="3"/>
-        <v>1455717.3529411764</v>
+        <f t="shared" si="4"/>
+        <v>1444168.1411764706</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="1"/>
-        <v>14651.934222770993</v>
+        <f t="shared" si="2"/>
+        <v>14652.008653386449</v>
       </c>
       <c r="K19" s="20">
-        <v>1237359.75</v>
+        <v>1227542.92</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.055711216724</v>
+        <f t="shared" si="3"/>
+        <v>13790.125875676984</v>
       </c>
       <c r="M19" s="20">
-        <v>1164573.8799999999</v>
+        <v>1155334.52</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B20" s="6">
-        <v>825</v>
+        <v>222</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
       </c>
       <c r="D20" s="6">
-        <v>65.150000000000006</v>
+        <v>66.69</v>
       </c>
       <c r="E20" s="7">
-        <v>17.38958354</v>
+        <v>17.760266509999997</v>
       </c>
       <c r="F20" s="7">
-        <v>82.53958354000001</v>
+        <v>84.450266509999992</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>17717.369144218424</v>
+        <v>17237.569673848226</v>
       </c>
       <c r="I20" s="20">
-        <f t="shared" si="3"/>
-        <v>1462384.2705882352</v>
+        <f t="shared" si="4"/>
+        <v>1455717.3529411764</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="1"/>
-        <v>15059.763772585662</v>
+        <f t="shared" si="2"/>
+        <v>14651.934222770993</v>
       </c>
       <c r="K20" s="20">
-        <v>1243026.6299999999</v>
+        <v>1237359.75</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="2"/>
-        <v>14173.895236980981</v>
+        <f t="shared" si="3"/>
+        <v>13790.055711216724</v>
       </c>
       <c r="M20" s="20">
-        <v>1169907.4099999999</v>
+        <v>1164573.8799999999</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B21" s="6">
-        <v>207</v>
+        <v>825</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
       </c>
       <c r="D21" s="6">
-        <v>66.010000000000005</v>
+        <v>65.150000000000006</v>
       </c>
       <c r="E21" s="7">
-        <v>9.0496812299999991</v>
+        <v>17.38958354</v>
       </c>
       <c r="F21" s="7">
-        <v>75.05968123000001</v>
+        <v>82.53958354000001</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>19486.092535296619</v>
+        <v>17717.369144218424</v>
       </c>
       <c r="I21" s="20">
-        <f t="shared" si="3"/>
-        <v>1462619.8941176469</v>
+        <f t="shared" si="4"/>
+        <v>1462384.2705882352</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.178655002128</v>
+        <f t="shared" si="2"/>
+        <v>15059.763772585662</v>
       </c>
       <c r="K21" s="20">
-        <v>1243226.9099999999</v>
+        <v>1243026.6299999999</v>
       </c>
       <c r="L21" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.874090932504</v>
+        <f t="shared" si="3"/>
+        <v>14173.895236980981</v>
       </c>
       <c r="M21" s="20">
-        <v>1170095.92</v>
+        <v>1169907.4099999999</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="6">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="D22" s="6">
-        <v>66.69</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="E22" s="7">
-        <v>18.390148849999999</v>
+        <v>9.0496812299999991</v>
       </c>
       <c r="F22" s="7">
-        <v>85.08014885</v>
+        <v>75.05968123000001</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>17237.593946963687</v>
+        <v>19486.092535296619</v>
       </c>
       <c r="I22" s="20">
-        <f t="shared" si="3"/>
-        <v>1466577.0588235294</v>
+        <f t="shared" si="4"/>
+        <v>1462619.8941176469</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="1"/>
-        <v>14651.954854919133</v>
+        <f t="shared" si="2"/>
+        <v>16563.178655002128</v>
       </c>
       <c r="K22" s="20">
-        <v>1246590.5</v>
+        <v>1243226.9099999999</v>
       </c>
       <c r="L22" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.075192140428</v>
+        <f t="shared" si="3"/>
+        <v>15588.874090932504</v>
       </c>
       <c r="M22" s="20">
-        <v>1173261.6499999999</v>
+        <v>1170095.92</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="6">
-        <v>217</v>
+        <v>122</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -1622,125 +1640,124 @@
         <v>66.69</v>
       </c>
       <c r="E23" s="7">
-        <v>19.020031189999997</v>
+        <v>18.390148849999999</v>
       </c>
       <c r="F23" s="7">
-        <v>85.710031189999995</v>
+        <v>85.08014885</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>17237.61786331328</v>
+        <v>17237.593946963687</v>
       </c>
       <c r="I23" s="20">
-        <f t="shared" si="3"/>
-        <v>1477436.7647058824</v>
+        <f t="shared" si="4"/>
+        <v>1466577.0588235294</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="1"/>
-        <v>14651.975183816288</v>
+        <f t="shared" si="2"/>
+        <v>14651.954854919133</v>
       </c>
       <c r="K23" s="20">
-        <v>1255821.25</v>
+        <v>1246590.5</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.094270061367</v>
+        <f t="shared" si="3"/>
+        <v>13790.075192140428</v>
       </c>
       <c r="M23" s="20">
-        <v>1181949.4099999999</v>
+        <v>1173261.6499999999</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B24" s="6">
-        <v>127</v>
+        <v>804</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
       <c r="D24" s="6">
-        <v>66.7</v>
-      </c>
-      <c r="E24" s="7">
-        <v>19.769758400000001</v>
-      </c>
-      <c r="F24" s="7">
-        <v>86.469758400000003</v>
+        <v>67.010000000000005</v>
+      </c>
+      <c r="E24" s="6">
+        <v>11.32</v>
+      </c>
+      <c r="F24" s="6">
+        <v>78.330000000000013</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>17237.672228088199</v>
-      </c>
-      <c r="I24" s="20">
-        <f t="shared" si="3"/>
-        <v>1490537.3529411764</v>
+        <v>18796.504832495997</v>
+      </c>
+      <c r="I24" s="22">
+        <v>1472330.2235294117</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="1"/>
-        <v>14652.021393874971</v>
+        <f t="shared" si="2"/>
+        <v>15977.029107621598</v>
       </c>
       <c r="K24" s="20">
-        <v>1266956.75</v>
+        <v>1251480.69</v>
       </c>
       <c r="L24" s="5">
-        <f t="shared" si="2"/>
-        <v>13790.137755259413</v>
-      </c>
-      <c r="M24" s="20">
-        <v>1192429.8799999999</v>
+        <f t="shared" si="3"/>
+        <v>15037.20388101621</v>
+      </c>
+      <c r="M24" s="23">
+        <v>1177864.18</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B25" s="6">
-        <v>827</v>
+        <v>217</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" s="6">
-        <v>66.7</v>
+        <v>66.69</v>
       </c>
       <c r="E25" s="7">
-        <v>18.700444869999998</v>
+        <v>19.020031189999997</v>
       </c>
       <c r="F25" s="7">
-        <v>85.400444870000001</v>
+        <v>85.710031189999995</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>17552.306692099788</v>
+        <v>17237.61786331328</v>
       </c>
       <c r="I25" s="20">
-        <f t="shared" si="3"/>
-        <v>1498974.8</v>
+        <f>(K25*100)/85</f>
+        <v>1477436.7647058824</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="1"/>
-        <v>14919.46068828482</v>
+        <f t="shared" si="2"/>
+        <v>14651.975183816288</v>
       </c>
       <c r="K25" s="20">
-        <v>1274128.58</v>
+        <v>1255821.25</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="2"/>
-        <v>14041.845353679832</v>
+        <f t="shared" si="3"/>
+        <v>13790.094270061367</v>
       </c>
       <c r="M25" s="20">
-        <v>1199179.8400000001</v>
+        <v>1181949.4099999999</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1748,494 +1765,491 @@
         <v>9</v>
       </c>
       <c r="B26" s="6">
-        <v>922</v>
+        <v>935</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" s="6">
-        <v>66.69</v>
-      </c>
-      <c r="E26" s="7">
-        <v>17.760266509999997</v>
-      </c>
-      <c r="F26" s="7">
-        <v>84.450266509999992</v>
+        <v>67.010000000000005</v>
+      </c>
+      <c r="E26" s="6">
+        <v>11.32</v>
+      </c>
+      <c r="F26" s="6">
+        <v>78.330000000000013</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>17762.191429228686</v>
-      </c>
-      <c r="I26" s="20">
-        <f t="shared" si="3"/>
-        <v>1500021.8</v>
+        <v>18886.440324118917</v>
+      </c>
+      <c r="I26" s="22">
+        <v>1479374.8705882351</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="1"/>
-        <v>15097.862714844381</v>
+        <f t="shared" si="2"/>
+        <v>16053.474275501081</v>
       </c>
       <c r="K26" s="20">
-        <v>1275018.53</v>
+        <v>1257468.6399999999</v>
       </c>
       <c r="L26" s="5">
-        <f t="shared" si="2"/>
-        <v>14209.753143382946</v>
-      </c>
-      <c r="M26" s="20">
-        <v>1200017.44</v>
+        <f t="shared" si="3"/>
+        <v>15109.152176688365</v>
+      </c>
+      <c r="M26" s="23">
+        <v>1183499.8899999999</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="6">
-        <v>830</v>
+        <v>603</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
       <c r="D27" s="6">
-        <v>68.77</v>
-      </c>
-      <c r="E27" s="7">
-        <v>19.219772639999999</v>
-      </c>
-      <c r="F27" s="7">
-        <v>87.989772639999998</v>
+        <v>68.05</v>
+      </c>
+      <c r="E27" s="6">
+        <v>11.81</v>
+      </c>
+      <c r="F27" s="6">
+        <v>79.86</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>17552.443420910207</v>
-      </c>
-      <c r="I27" s="20">
-        <f t="shared" si="3"/>
-        <v>1544435.5058823531</v>
+        <v>18661.601773692197</v>
+      </c>
+      <c r="I27" s="22">
+        <v>1490315.5176470589</v>
       </c>
       <c r="J27" s="5">
-        <f t="shared" si="1"/>
-        <v>14919.576907773675</v>
+        <f t="shared" si="2"/>
+        <v>15862.361507638367</v>
       </c>
       <c r="K27" s="20">
-        <v>1312770.18</v>
+        <v>1266768.19</v>
       </c>
       <c r="L27" s="5">
-        <f t="shared" si="2"/>
-        <v>14041.954796895585</v>
-      </c>
-      <c r="M27" s="20">
-        <v>1235548.4099999999</v>
+        <f t="shared" si="3"/>
+        <v>14929.281367392936</v>
+      </c>
+      <c r="M27" s="23">
+        <v>1192252.4099999999</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="6">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
       <c r="D28" s="6">
-        <v>68.05</v>
+        <v>66.7</v>
       </c>
       <c r="E28" s="7">
-        <v>11.80982936</v>
+        <v>19.769758400000001</v>
       </c>
       <c r="F28" s="7">
-        <v>79.859829359999992</v>
+        <v>86.469758400000003</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>19486.051418435822</v>
+        <v>17237.672228088199</v>
       </c>
       <c r="I28" s="20">
-        <f t="shared" si="3"/>
-        <v>1556152.7411764706</v>
+        <f>(K28*100)/85</f>
+        <v>1490537.3529411764</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.143705670449</v>
+        <f t="shared" si="2"/>
+        <v>14652.021393874971</v>
       </c>
       <c r="K28" s="20">
-        <v>1322729.83</v>
+        <v>1266956.75</v>
       </c>
       <c r="L28" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.841223138823</v>
+        <f t="shared" si="3"/>
+        <v>13790.137755259413</v>
       </c>
       <c r="M28" s="20">
-        <v>1244922.2</v>
+        <v>1192429.8799999999</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B29" s="6">
-        <v>108</v>
+        <v>829</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="6">
-        <v>65.75</v>
-      </c>
-      <c r="E29" s="7">
-        <v>25.220377410000001</v>
-      </c>
-      <c r="F29" s="7">
-        <v>90.970377409999998</v>
+        <v>68.83</v>
+      </c>
+      <c r="E29" s="6">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="F29" s="6">
+        <v>85.09</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>19485.929025641257</v>
-      </c>
-      <c r="I29" s="20">
-        <f t="shared" si="3"/>
-        <v>1772642.3176470587</v>
+        <v>17552.398083689935</v>
+      </c>
+      <c r="I29" s="22">
+        <v>1493533.5529411766</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.039671795068</v>
+        <f t="shared" si="2"/>
+        <v>14919.538371136443</v>
       </c>
       <c r="K29" s="20">
-        <v>1506745.97</v>
+        <v>1269503.52</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.743175249405</v>
-      </c>
-      <c r="M29" s="20">
-        <v>1418113.85</v>
+        <f t="shared" si="3"/>
+        <v>14041.918439299565</v>
+      </c>
+      <c r="M29" s="23">
+        <v>1194826.8400000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B30" s="6">
-        <v>107</v>
+        <v>827</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
       </c>
       <c r="D30" s="6">
-        <v>66.010000000000005</v>
+        <v>66.7</v>
       </c>
       <c r="E30" s="7">
-        <v>25.500015440000002</v>
+        <v>18.700444869999998</v>
       </c>
       <c r="F30" s="7">
-        <v>91.510015440000004</v>
+        <v>85.400444870000001</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>19486.006598644308</v>
+        <v>17552.306692099788</v>
       </c>
       <c r="I30" s="20">
-        <f t="shared" si="3"/>
-        <v>1783164.7647058824</v>
+        <f t="shared" ref="I30:I46" si="5">(K30*100)/85</f>
+        <v>1498974.8</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.105608847662</v>
+        <f t="shared" si="2"/>
+        <v>14919.46068828482</v>
       </c>
       <c r="K30" s="20">
-        <v>1515690.05</v>
+        <v>1274128.58</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.805259631154</v>
+        <f t="shared" si="3"/>
+        <v>14041.845353679832</v>
       </c>
       <c r="M30" s="20">
-        <v>1426531.81</v>
+        <v>1199179.8400000001</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B31" s="6">
-        <v>132</v>
+        <v>922</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
       </c>
       <c r="D31" s="6">
-        <v>66.010000000000005</v>
+        <v>66.69</v>
       </c>
       <c r="E31" s="7">
-        <v>25.500015440000002</v>
+        <v>17.760266509999997</v>
       </c>
       <c r="F31" s="7">
-        <v>91.510015440000004</v>
+        <v>84.450266509999992</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>19486.006598644308</v>
+        <v>17762.191429228686</v>
       </c>
       <c r="I31" s="20">
-        <f t="shared" si="3"/>
-        <v>1783164.7647058824</v>
+        <f t="shared" si="5"/>
+        <v>1500021.8</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.105608847662</v>
+        <f t="shared" si="2"/>
+        <v>15097.862714844381</v>
       </c>
       <c r="K31" s="20">
-        <v>1515690.05</v>
+        <v>1275018.53</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.805259631154</v>
+        <f t="shared" si="3"/>
+        <v>14209.753143382946</v>
       </c>
       <c r="M31" s="20">
-        <v>1426531.81</v>
+        <v>1200017.44</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B32" s="6">
-        <v>103</v>
+        <v>830</v>
       </c>
       <c r="C32" s="6">
         <v>1</v>
       </c>
       <c r="D32" s="6">
-        <v>68.05</v>
+        <v>68.77</v>
       </c>
       <c r="E32" s="7">
-        <v>25.319783620000003</v>
+        <v>19.219772639999999</v>
       </c>
       <c r="F32" s="7">
-        <v>93.369783619999993</v>
+        <v>87.989772639999998</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>19486.055023766272</v>
+        <v>17552.443420910207</v>
       </c>
       <c r="I32" s="20">
-        <f t="shared" si="3"/>
-        <v>1819408.7411764706</v>
+        <f t="shared" si="5"/>
+        <v>1544435.5058823531</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.146770201329</v>
+        <f t="shared" si="2"/>
+        <v>14919.576907773675</v>
       </c>
       <c r="K32" s="20">
-        <v>1546497.43</v>
+        <v>1312770.18</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.843987512713</v>
+        <f t="shared" si="3"/>
+        <v>14041.954796895585</v>
       </c>
       <c r="M32" s="20">
-        <v>1455526.99</v>
+        <v>1235548.4099999999</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B33" s="6">
-        <v>1011</v>
+        <v>203</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
       <c r="D33" s="6">
-        <v>73.31</v>
+        <v>68.05</v>
       </c>
       <c r="E33" s="7">
-        <v>42.609960949999994</v>
+        <v>11.80982936</v>
       </c>
       <c r="F33" s="7">
-        <v>115.91996094999999</v>
+        <v>79.859829359999992</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>16038.490463581322</v>
+        <v>19486.051418435822</v>
       </c>
       <c r="I33" s="20">
-        <f t="shared" si="3"/>
-        <v>1859181.1882352941</v>
+        <f t="shared" si="5"/>
+        <v>1556152.7411764706</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="1"/>
-        <v>13632.716894044124</v>
+        <f t="shared" si="2"/>
+        <v>16563.143705670449</v>
       </c>
       <c r="K33" s="20">
-        <v>1580304.01</v>
+        <v>1322729.83</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="2"/>
-        <v>12830.792365790563</v>
+        <f t="shared" si="3"/>
+        <v>15588.841223138823</v>
       </c>
       <c r="M33" s="20">
-        <v>1487344.95</v>
+        <v>1244922.2</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B34" s="6">
-        <v>1017</v>
+        <v>108</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
       </c>
       <c r="D34" s="6">
-        <v>73.31</v>
+        <v>65.75</v>
       </c>
       <c r="E34" s="7">
-        <v>47.500374870000002</v>
+        <v>25.220377410000001</v>
       </c>
       <c r="F34" s="7">
-        <v>120.81037487</v>
+        <v>90.970377409999998</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>15738.651407353158</v>
+        <v>19485.929025641257</v>
       </c>
       <c r="I34" s="20">
-        <f t="shared" si="3"/>
-        <v>1901392.3764705881</v>
+        <f t="shared" si="5"/>
+        <v>1772642.3176470587</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="1"/>
-        <v>13377.853696250186</v>
+        <f t="shared" si="2"/>
+        <v>16563.039671795068</v>
       </c>
       <c r="K34" s="20">
-        <v>1616183.52</v>
+        <v>1506745.97</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="2"/>
-        <v>12590.921116144367</v>
+        <f t="shared" si="3"/>
+        <v>15588.743175249405</v>
       </c>
       <c r="M34" s="20">
-        <v>1521113.9</v>
+        <v>1418113.85</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B35" s="6">
-        <v>1016</v>
+        <v>107</v>
       </c>
       <c r="C35" s="6">
         <v>1</v>
       </c>
       <c r="D35" s="6">
-        <v>73.400000000000006</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="E35" s="7">
-        <v>56.149644170000002</v>
+        <v>25.500015440000002</v>
       </c>
       <c r="F35" s="7">
-        <v>129.54964417000002</v>
+        <v>91.510015440000004</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>14989.279484096722</v>
+        <v>19486.006598644308</v>
       </c>
       <c r="I35" s="20">
-        <f t="shared" si="3"/>
-        <v>1941855.8235294118</v>
+        <f t="shared" si="5"/>
+        <v>1783164.7647058824</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="1"/>
-        <v>12740.887561482214</v>
+        <f t="shared" si="2"/>
+        <v>16563.105608847662</v>
       </c>
       <c r="K35" s="20">
-        <v>1650577.45</v>
+        <v>1515690.05</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="2"/>
-        <v>11991.423596358611</v>
+        <f t="shared" si="3"/>
+        <v>15588.805259631154</v>
       </c>
       <c r="M35" s="20">
-        <v>1553484.66</v>
+        <v>1426531.81</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B36" s="6">
-        <v>1010</v>
+        <v>132</v>
       </c>
       <c r="C36" s="6">
         <v>1</v>
       </c>
       <c r="D36" s="6">
-        <v>73.400000000000006</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="E36" s="7">
-        <v>50.380367869999994</v>
+        <v>25.500015440000002</v>
       </c>
       <c r="F36" s="7">
-        <v>123.78036786999999</v>
+        <v>91.510015440000004</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>15738.653480922627</v>
+        <v>19486.006598644308</v>
       </c>
       <c r="I36" s="20">
-        <f t="shared" si="3"/>
-        <v>1948136.3176470587</v>
+        <f t="shared" si="5"/>
+        <v>1783164.7647058824</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="1"/>
-        <v>13377.855458784235</v>
+        <f t="shared" si="2"/>
+        <v>16563.105608847662</v>
       </c>
       <c r="K36" s="20">
-        <v>1655915.87</v>
+        <v>1515690.05</v>
       </c>
       <c r="L36" s="5">
-        <f t="shared" si="2"/>
-        <v>12590.92275147235</v>
+        <f t="shared" si="3"/>
+        <v>15588.805259631154</v>
       </c>
       <c r="M36" s="20">
-        <v>1558509.05</v>
+        <v>1426531.81</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2243,539 +2257,538 @@
         <v>1</v>
       </c>
       <c r="B37" s="6">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="6">
         <v>1</v>
       </c>
       <c r="D37" s="6">
-        <v>74.72</v>
+        <v>68.05</v>
       </c>
       <c r="E37" s="7">
-        <v>26.910282980000002</v>
+        <v>25.319783620000003</v>
       </c>
       <c r="F37" s="7">
-        <v>101.63028298</v>
+        <v>93.369783619999993</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>19485.955547917813</v>
+        <v>19486.055023766272</v>
       </c>
       <c r="I37" s="20">
-        <f t="shared" si="3"/>
-        <v>1980363.1764705882</v>
+        <f t="shared" si="5"/>
+        <v>1819408.7411764706</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="1"/>
-        <v>16563.06221573014</v>
+        <f t="shared" si="2"/>
+        <v>16563.146770201329</v>
       </c>
       <c r="K37" s="20">
-        <v>1683308.7</v>
+        <v>1546497.43</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" si="2"/>
-        <v>15588.764426758265</v>
+        <f t="shared" si="3"/>
+        <v>15588.843987512713</v>
       </c>
       <c r="M37" s="20">
-        <v>1584290.54</v>
+        <v>1455526.99</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B38" s="6">
-        <v>238</v>
+        <v>1011</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
       <c r="D38" s="6">
-        <v>73.56</v>
+        <v>73.31</v>
       </c>
       <c r="E38" s="7">
-        <v>37.120322680000001</v>
+        <v>42.609960949999994</v>
       </c>
       <c r="F38" s="7">
-        <v>110.68032268</v>
+        <v>115.91996094999999</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>17987.033595021148</v>
+        <v>16038.490463581322</v>
       </c>
       <c r="I38" s="20">
-        <f t="shared" si="3"/>
-        <v>1990810.6823529413</v>
+        <f t="shared" si="5"/>
+        <v>1859181.1882352941</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="1"/>
-        <v>15288.978555767977</v>
+        <f t="shared" si="2"/>
+        <v>13632.716894044124</v>
       </c>
       <c r="K38" s="20">
-        <v>1692189.08</v>
+        <v>1580304.01</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="2"/>
-        <v>14389.626822869686</v>
+        <f t="shared" si="3"/>
+        <v>12830.792365790563</v>
       </c>
       <c r="M38" s="20">
-        <v>1592648.54</v>
+        <v>1487344.95</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
+        <v>10</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1017</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1</v>
+      </c>
+      <c r="D39" s="6">
+        <v>73.31</v>
+      </c>
+      <c r="E39" s="7">
+        <v>47.500374870000002</v>
+      </c>
+      <c r="F39" s="7">
+        <v>120.81037487</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="0"/>
+        <v>15738.651407353158</v>
+      </c>
+      <c r="I39" s="20">
+        <f t="shared" si="5"/>
+        <v>1901392.3764705881</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="2"/>
+        <v>13377.853696250186</v>
+      </c>
+      <c r="K39" s="20">
+        <v>1616183.52</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" si="3"/>
+        <v>12590.921116144367</v>
+      </c>
+      <c r="M39" s="20">
+        <v>1521113.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>10</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1016</v>
+      </c>
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
+      <c r="D40" s="6">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="E40" s="7">
+        <v>56.149644170000002</v>
+      </c>
+      <c r="F40" s="7">
+        <v>129.54964417000002</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="0"/>
+        <v>14989.279484096722</v>
+      </c>
+      <c r="I40" s="20">
+        <f t="shared" si="5"/>
+        <v>1941855.8235294118</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="2"/>
+        <v>12740.887561482214</v>
+      </c>
+      <c r="K40" s="20">
+        <v>1650577.45</v>
+      </c>
+      <c r="L40" s="5">
+        <f t="shared" si="3"/>
+        <v>11991.423596358611</v>
+      </c>
+      <c r="M40" s="20">
+        <v>1553484.66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>10</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1010</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="E41" s="7">
+        <v>50.380367869999994</v>
+      </c>
+      <c r="F41" s="7">
+        <v>123.78036786999999</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="0"/>
+        <v>15738.653480922627</v>
+      </c>
+      <c r="I41" s="20">
+        <f t="shared" si="5"/>
+        <v>1948136.3176470587</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="2"/>
+        <v>13377.855458784235</v>
+      </c>
+      <c r="K41" s="20">
+        <v>1655915.87</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" si="3"/>
+        <v>12590.92275147235</v>
+      </c>
+      <c r="M41" s="20">
+        <v>1558509.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>1</v>
+      </c>
+      <c r="B42" s="6">
+        <v>102</v>
+      </c>
+      <c r="C42" s="6">
+        <v>1</v>
+      </c>
+      <c r="D42" s="6">
+        <v>74.72</v>
+      </c>
+      <c r="E42" s="7">
+        <v>26.910282980000002</v>
+      </c>
+      <c r="F42" s="7">
+        <v>101.63028298</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" si="0"/>
+        <v>19485.955547917813</v>
+      </c>
+      <c r="I42" s="20">
+        <f t="shared" si="5"/>
+        <v>1980363.1764705882</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="2"/>
+        <v>16563.06221573014</v>
+      </c>
+      <c r="K42" s="20">
+        <v>1683308.7</v>
+      </c>
+      <c r="L42" s="5">
+        <f t="shared" si="3"/>
+        <v>15588.764426758265</v>
+      </c>
+      <c r="M42" s="20">
+        <v>1584290.54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
         <v>2</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B43" s="6">
+        <v>238</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6">
+        <v>73.56</v>
+      </c>
+      <c r="E43" s="7">
+        <v>37.120322680000001</v>
+      </c>
+      <c r="F43" s="7">
+        <v>110.68032268</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="0"/>
+        <v>17987.033595021148</v>
+      </c>
+      <c r="I43" s="20">
+        <f t="shared" si="5"/>
+        <v>1990810.6823529413</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="2"/>
+        <v>15288.978555767977</v>
+      </c>
+      <c r="K43" s="20">
+        <v>1692189.08</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" si="3"/>
+        <v>14389.626822869686</v>
+      </c>
+      <c r="M43" s="20">
+        <v>1592648.54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>2</v>
+      </c>
+      <c r="B44" s="6">
         <v>201</v>
       </c>
-      <c r="C39" s="6">
-        <v>1</v>
-      </c>
-      <c r="D39" s="6">
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6">
         <v>73.56</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E44" s="7">
         <v>37.33957376</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F44" s="7">
         <v>110.89957376000001</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H44" s="5">
         <f t="shared" si="0"/>
         <v>17987.155113968562</v>
       </c>
-      <c r="I39" s="20">
-        <f t="shared" si="3"/>
+      <c r="I44" s="20">
+        <f t="shared" si="5"/>
         <v>1994767.8352941177</v>
       </c>
-      <c r="J39" s="5">
-        <f t="shared" si="1"/>
+      <c r="J44" s="5">
+        <f t="shared" si="2"/>
         <v>15289.081846873274</v>
       </c>
-      <c r="K39" s="20">
+      <c r="K44" s="20">
         <v>1695552.66</v>
       </c>
-      <c r="L39" s="5">
-        <f t="shared" si="2"/>
+      <c r="L44" s="5">
+        <f t="shared" si="3"/>
         <v>14389.724107087495</v>
       </c>
-      <c r="M39" s="20">
+      <c r="M44" s="20">
         <v>1595814.27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="8">
-        <v>4</v>
-      </c>
-      <c r="B40" s="8">
-        <v>419</v>
-      </c>
-      <c r="C40" s="8">
-        <v>2</v>
-      </c>
-      <c r="D40" s="8">
-        <v>87.87</v>
-      </c>
-      <c r="E40" s="9">
-        <v>15.340143360000001</v>
-      </c>
-      <c r="F40" s="9">
-        <v>103.21014336</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="10">
-        <f t="shared" si="0"/>
-        <v>19560.928847335294</v>
-      </c>
-      <c r="I40" s="21">
-        <f t="shared" si="3"/>
-        <v>2018886.2705882352</v>
-      </c>
-      <c r="J40" s="10">
-        <f t="shared" si="1"/>
-        <v>16626.789520235001</v>
-      </c>
-      <c r="K40" s="21">
-        <v>1716053.33</v>
-      </c>
-      <c r="L40" s="10">
-        <f t="shared" si="2"/>
-        <v>15648.7431120646</v>
-      </c>
-      <c r="M40" s="21">
-        <v>1615109.02</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="8">
-        <v>5</v>
-      </c>
-      <c r="B41" s="8">
-        <v>519</v>
-      </c>
-      <c r="C41" s="8">
-        <v>2</v>
-      </c>
-      <c r="D41" s="8">
-        <v>87.87</v>
-      </c>
-      <c r="E41" s="9">
-        <v>15.340143360000001</v>
-      </c>
-      <c r="F41" s="9">
-        <v>103.21014336</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="10">
-        <f t="shared" si="0"/>
-        <v>19620.885676574373</v>
-      </c>
-      <c r="I41" s="21">
-        <f t="shared" si="3"/>
-        <v>2025074.4235294117</v>
-      </c>
-      <c r="J41" s="10">
-        <f t="shared" si="1"/>
-        <v>16677.752825088217</v>
-      </c>
-      <c r="K41" s="21">
-        <v>1721313.26</v>
-      </c>
-      <c r="L41" s="10">
-        <f t="shared" si="2"/>
-        <v>15696.708552658287</v>
-      </c>
-      <c r="M41" s="21">
-        <v>1620059.54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="8">
-        <v>8</v>
-      </c>
-      <c r="B42" s="8">
-        <v>820</v>
-      </c>
-      <c r="C42" s="8">
-        <v>2</v>
-      </c>
-      <c r="D42" s="8">
-        <v>87.87</v>
-      </c>
-      <c r="E42" s="9">
-        <v>16.599908039999999</v>
-      </c>
-      <c r="F42" s="9">
-        <v>104.46990804000001</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="10">
-        <f t="shared" si="0"/>
-        <v>19800.801217905821</v>
-      </c>
-      <c r="I42" s="21">
-        <f t="shared" si="3"/>
-        <v>2068587.8823529412</v>
-      </c>
-      <c r="J42" s="10">
-        <f t="shared" si="1"/>
-        <v>16830.681035219946</v>
-      </c>
-      <c r="K42" s="21">
-        <v>1758299.7</v>
-      </c>
-      <c r="L42" s="10">
-        <f t="shared" si="2"/>
-        <v>15840.641013739329</v>
-      </c>
-      <c r="M42" s="21">
-        <v>1654870.31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="8">
-        <v>4</v>
-      </c>
-      <c r="B43" s="8">
-        <v>420</v>
-      </c>
-      <c r="C43" s="8">
-        <v>2</v>
-      </c>
-      <c r="D43" s="8">
-        <v>87.87</v>
-      </c>
-      <c r="E43" s="9">
-        <v>19.51984933</v>
-      </c>
-      <c r="F43" s="9">
-        <v>107.38984933</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="10">
-        <f t="shared" si="0"/>
-        <v>19560.983497919908</v>
-      </c>
-      <c r="I43" s="21">
-        <f t="shared" si="3"/>
-        <v>2100651.0705882353</v>
-      </c>
-      <c r="J43" s="10">
-        <f t="shared" si="1"/>
-        <v>16626.835973231919</v>
-      </c>
-      <c r="K43" s="21">
-        <v>1785553.41</v>
-      </c>
-      <c r="L43" s="10">
-        <f t="shared" si="2"/>
-        <v>15648.78673808267</v>
-      </c>
-      <c r="M43" s="21">
-        <v>1680520.85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="8">
-        <v>10</v>
-      </c>
-      <c r="B44" s="8">
-        <v>1005</v>
-      </c>
-      <c r="C44" s="8">
-        <v>2</v>
-      </c>
-      <c r="D44" s="8">
-        <v>87.87</v>
-      </c>
-      <c r="E44" s="9">
-        <v>19.51984933</v>
-      </c>
-      <c r="F44" s="9">
-        <v>107.38984933</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="10">
-        <f t="shared" si="0"/>
-        <v>20235.500090931666</v>
-      </c>
-      <c r="I44" s="21">
-        <f t="shared" si="3"/>
-        <v>2173087.3058823529</v>
-      </c>
-      <c r="J44" s="10">
-        <f t="shared" si="1"/>
-        <v>17200.175077291915</v>
-      </c>
-      <c r="K44" s="21">
-        <v>1847124.21</v>
-      </c>
-      <c r="L44" s="10">
-        <f t="shared" si="2"/>
-        <v>16188.400122043453</v>
-      </c>
-      <c r="M44" s="21">
-        <v>1738469.85</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B45" s="8">
-        <v>1006</v>
+        <v>419</v>
       </c>
       <c r="C45" s="8">
         <v>2</v>
       </c>
       <c r="D45" s="8">
-        <v>88.13</v>
+        <v>87.87</v>
       </c>
       <c r="E45" s="9">
-        <v>57.209667399999994</v>
+        <v>15.340143360000001</v>
       </c>
       <c r="F45" s="9">
-        <v>145.3396674</v>
+        <v>103.21014336</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H45" s="10">
         <f t="shared" si="0"/>
-        <v>14989.272599076052</v>
+        <v>19560.928847335294</v>
       </c>
       <c r="I45" s="21">
-        <f t="shared" si="3"/>
-        <v>2178535.8941176469</v>
+        <f t="shared" si="5"/>
+        <v>2018886.2705882352</v>
       </c>
       <c r="J45" s="10">
-        <f t="shared" si="1"/>
-        <v>12740.881709214646</v>
+        <f t="shared" si="2"/>
+        <v>16626.789520235001</v>
       </c>
       <c r="K45" s="21">
-        <v>1851755.51</v>
+        <v>1716053.33</v>
       </c>
       <c r="L45" s="10">
-        <f t="shared" si="2"/>
-        <v>11991.418111639356</v>
+        <f t="shared" si="3"/>
+        <v>15648.7431120646</v>
       </c>
       <c r="M45" s="21">
-        <v>1742828.72</v>
+        <v>1615109.02</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B46" s="8">
-        <v>818</v>
+        <v>519</v>
       </c>
       <c r="C46" s="8">
         <v>2</v>
       </c>
       <c r="D46" s="8">
-        <v>88.01</v>
+        <v>87.87</v>
       </c>
       <c r="E46" s="9">
-        <v>23.400407640000001</v>
+        <v>15.340143360000001</v>
       </c>
       <c r="F46" s="9">
-        <v>111.41040764</v>
+        <v>103.21014336</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="10">
         <f t="shared" si="0"/>
-        <v>19800.711406963168</v>
+        <v>19620.885676574373</v>
       </c>
       <c r="I46" s="21">
-        <f t="shared" si="3"/>
-        <v>2206005.3294117646</v>
+        <f t="shared" si="5"/>
+        <v>2025074.4235294117</v>
       </c>
       <c r="J46" s="10">
-        <f t="shared" si="1"/>
-        <v>16830.604695918693</v>
+        <f t="shared" si="2"/>
+        <v>16677.752825088217</v>
       </c>
       <c r="K46" s="21">
-        <v>1875104.53</v>
+        <v>1721313.26</v>
       </c>
       <c r="L46" s="10">
-        <f t="shared" si="2"/>
-        <v>15840.569093891163</v>
+        <f t="shared" si="3"/>
+        <v>15696.708552658287</v>
       </c>
       <c r="M46" s="21">
-        <v>1764804.26</v>
+        <v>1620059.54</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B47" s="8">
-        <v>1003</v>
+        <v>819</v>
       </c>
       <c r="C47" s="8">
         <v>2</v>
       </c>
       <c r="D47" s="8">
-        <v>88.08</v>
-      </c>
-      <c r="E47" s="9">
-        <v>59.509945679999994</v>
-      </c>
-      <c r="F47" s="9">
-        <v>147.58994568</v>
+        <v>87.87</v>
+      </c>
+      <c r="E47" s="8">
+        <v>15.92</v>
+      </c>
+      <c r="F47" s="8">
+        <v>103.79</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H47" s="10">
         <f t="shared" si="0"/>
-        <v>14989.243827960334</v>
-      </c>
-      <c r="I47" s="21">
-        <f t="shared" si="3"/>
-        <v>2212261.682352941</v>
+        <v>19800.783822537589</v>
+      </c>
+      <c r="I47" s="24">
+        <v>2055123.3529411764</v>
       </c>
       <c r="J47" s="10">
-        <f t="shared" si="1"/>
-        <v>12740.857253766284</v>
+        <f t="shared" si="2"/>
+        <v>16830.666249156951</v>
       </c>
       <c r="K47" s="21">
-        <v>1880422.43</v>
+        <v>1746854.85</v>
       </c>
       <c r="L47" s="10">
-        <f t="shared" si="2"/>
-        <v>11991.395090267508</v>
-      </c>
-      <c r="M47" s="21">
-        <v>1769809.35</v>
+        <f t="shared" si="3"/>
+        <v>15840.627035359859</v>
+      </c>
+      <c r="M47" s="25">
+        <v>1644098.68</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B48" s="8">
-        <v>211</v>
+        <v>820</v>
       </c>
       <c r="C48" s="8">
         <v>2</v>
       </c>
       <c r="D48" s="8">
-        <v>96.66</v>
+        <v>87.87</v>
       </c>
       <c r="E48" s="9">
-        <v>17.630202310000001</v>
+        <v>16.599908039999999</v>
       </c>
       <c r="F48" s="9">
-        <v>114.29020231</v>
+        <v>104.46990804000001</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H48" s="10">
         <f t="shared" si="0"/>
-        <v>19485.975296315228</v>
+        <v>19800.801217905821</v>
       </c>
       <c r="I48" s="21">
-        <f t="shared" si="3"/>
-        <v>2227056.0588235296</v>
+        <f t="shared" ref="I48:I62" si="6">(K48*100)/85</f>
+        <v>2068587.8823529412</v>
       </c>
       <c r="J48" s="10">
-        <f t="shared" si="1"/>
-        <v>16563.079001867944</v>
+        <f t="shared" si="2"/>
+        <v>16830.681035219946</v>
       </c>
       <c r="K48" s="21">
-        <v>1892997.65</v>
+        <v>1758299.7</v>
       </c>
       <c r="L48" s="10">
-        <f t="shared" si="2"/>
-        <v>15588.780262786466</v>
+        <f t="shared" si="3"/>
+        <v>15840.641013739329</v>
       </c>
       <c r="M48" s="21">
-        <v>1781644.85</v>
+        <v>1654870.31</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -2783,269 +2796,269 @@
         <v>4</v>
       </c>
       <c r="B49" s="8">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C49" s="8">
         <v>2</v>
       </c>
       <c r="D49" s="8">
-        <v>96.69</v>
+        <v>87.87</v>
       </c>
       <c r="E49" s="9">
-        <v>20.199899290000001</v>
+        <v>19.51984933</v>
       </c>
       <c r="F49" s="9">
-        <v>116.88989929</v>
+        <v>107.38984933</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H49" s="10">
         <f t="shared" si="0"/>
-        <v>19560.972905524493</v>
+        <v>19560.983497919908</v>
       </c>
       <c r="I49" s="21">
-        <f t="shared" si="3"/>
-        <v>2286480.1529411767</v>
+        <f t="shared" si="6"/>
+        <v>2100651.0705882353</v>
       </c>
       <c r="J49" s="10">
-        <f t="shared" si="1"/>
-        <v>16626.826969695816</v>
+        <f t="shared" si="2"/>
+        <v>16626.835973231919</v>
       </c>
       <c r="K49" s="21">
-        <v>1943508.13</v>
+        <v>1785553.41</v>
       </c>
       <c r="L49" s="10">
-        <f t="shared" si="2"/>
-        <v>15648.778304290043</v>
+        <f t="shared" si="3"/>
+        <v>15648.78673808267</v>
       </c>
       <c r="M49" s="21">
-        <v>1829184.12</v>
+        <v>1680520.85</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B50" s="8">
-        <v>528</v>
+        <v>1005</v>
       </c>
       <c r="C50" s="8">
         <v>2</v>
       </c>
       <c r="D50" s="8">
-        <v>96.69</v>
+        <v>87.87</v>
       </c>
       <c r="E50" s="9">
-        <v>20.199899290000001</v>
+        <v>19.51984933</v>
       </c>
       <c r="F50" s="9">
-        <v>116.88989929</v>
+        <v>107.38984933</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H50" s="10">
         <f t="shared" si="0"/>
-        <v>19620.929879980384</v>
+        <v>20235.500090931666</v>
       </c>
       <c r="I50" s="21">
-        <f t="shared" si="3"/>
-        <v>2293488.5176470587</v>
+        <f t="shared" si="6"/>
+        <v>2173087.3058823529</v>
       </c>
       <c r="J50" s="10">
-        <f t="shared" si="1"/>
-        <v>16677.790397983325</v>
+        <f t="shared" si="2"/>
+        <v>17200.175077291915</v>
       </c>
       <c r="K50" s="21">
-        <v>1949465.24</v>
+        <v>1847124.21</v>
       </c>
       <c r="L50" s="10">
-        <f t="shared" si="2"/>
-        <v>15696.743868757592</v>
+        <f t="shared" si="3"/>
+        <v>16188.400122043453</v>
       </c>
       <c r="M50" s="21">
-        <v>1834790.81</v>
+        <v>1738469.85</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B51" s="8">
-        <v>311</v>
+        <v>1006</v>
       </c>
       <c r="C51" s="8">
         <v>2</v>
       </c>
       <c r="D51" s="8">
-        <v>96.66</v>
+        <v>88.13</v>
       </c>
       <c r="E51" s="9">
-        <v>17.630202310000001</v>
+        <v>57.209667399999994</v>
       </c>
       <c r="F51" s="9">
-        <v>114.29020231</v>
+        <v>145.3396674</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H51" s="10">
         <f t="shared" si="0"/>
-        <v>20818.285476211349</v>
+        <v>14989.272599076052</v>
       </c>
       <c r="I51" s="21">
-        <f t="shared" si="3"/>
-        <v>2379326.0588235296</v>
+        <f t="shared" si="6"/>
+        <v>2178535.8941176469</v>
       </c>
       <c r="J51" s="10">
-        <f t="shared" si="1"/>
-        <v>17695.542654779645</v>
+        <f t="shared" si="2"/>
+        <v>12740.881709214646</v>
       </c>
       <c r="K51" s="21">
-        <v>2022427.15</v>
+        <v>1851755.51</v>
       </c>
       <c r="L51" s="10">
-        <f t="shared" si="2"/>
-        <v>16654.628406703363</v>
+        <f t="shared" si="3"/>
+        <v>11991.418111639356</v>
       </c>
       <c r="M51" s="21">
-        <v>1903460.85</v>
+        <v>1742828.72</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B52" s="8">
-        <v>628</v>
+        <v>818</v>
       </c>
       <c r="C52" s="8">
         <v>2</v>
       </c>
       <c r="D52" s="8">
-        <v>96.69</v>
+        <v>88.01</v>
       </c>
       <c r="E52" s="9">
-        <v>24.43999221</v>
+        <v>23.400407640000001</v>
       </c>
       <c r="F52" s="9">
-        <v>121.12999221</v>
+        <v>111.41040764</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H52" s="10">
         <f t="shared" si="0"/>
-        <v>19680.871210968173</v>
+        <v>19800.711406963168</v>
       </c>
       <c r="I52" s="21">
-        <f t="shared" si="3"/>
-        <v>2383943.7764705881</v>
+        <f t="shared" si="6"/>
+        <v>2206005.3294117646</v>
       </c>
       <c r="J52" s="10">
-        <f t="shared" si="1"/>
-        <v>16728.740529322949</v>
+        <f t="shared" si="2"/>
+        <v>16830.604695918693</v>
       </c>
       <c r="K52" s="21">
-        <v>2026352.21</v>
+        <v>1875104.53</v>
       </c>
       <c r="L52" s="10">
-        <f t="shared" si="2"/>
-        <v>15744.696959062077</v>
+        <f t="shared" si="3"/>
+        <v>15840.569093891163</v>
       </c>
       <c r="M52" s="21">
-        <v>1907155.02</v>
+        <v>1764804.26</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B53" s="8">
-        <v>828</v>
+        <v>1003</v>
       </c>
       <c r="C53" s="8">
         <v>2</v>
       </c>
       <c r="D53" s="8">
-        <v>96.69</v>
+        <v>88.08</v>
       </c>
       <c r="E53" s="9">
-        <v>24.43999221</v>
+        <v>59.509945679999994</v>
       </c>
       <c r="F53" s="9">
-        <v>121.12999221</v>
+        <v>147.58994568</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H53" s="10">
         <f t="shared" si="0"/>
-        <v>19800.785069137175</v>
+        <v>14989.243827960334</v>
       </c>
       <c r="I53" s="21">
-        <f t="shared" si="3"/>
-        <v>2398468.9411764704</v>
+        <f t="shared" si="6"/>
+        <v>2212261.682352941</v>
       </c>
       <c r="J53" s="10">
-        <f t="shared" si="1"/>
-        <v>16830.667308766602</v>
+        <f t="shared" si="2"/>
+        <v>12740.857253766284</v>
       </c>
       <c r="K53" s="21">
-        <v>2038698.6</v>
+        <v>1880422.43</v>
       </c>
       <c r="L53" s="10">
-        <f t="shared" si="2"/>
-        <v>15840.62811358452</v>
+        <f t="shared" si="3"/>
+        <v>11991.395090267508</v>
       </c>
       <c r="M53" s="21">
-        <v>1918775.16</v>
+        <v>1769809.35</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B54" s="8">
-        <v>326</v>
+        <v>211</v>
       </c>
       <c r="C54" s="8">
         <v>2</v>
       </c>
       <c r="D54" s="8">
-        <v>112.4</v>
+        <v>96.66</v>
       </c>
       <c r="E54" s="9">
-        <v>56.720068589999997</v>
+        <v>17.630202310000001</v>
       </c>
       <c r="F54" s="9">
-        <v>169.12006859000002</v>
+        <v>114.29020231</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H54" s="10">
-        <f t="shared" ref="H54:H56" si="4">I54/F54</f>
-        <v>16787.940141618259</v>
+        <f t="shared" si="0"/>
+        <v>19485.975296315228</v>
       </c>
       <c r="I54" s="21">
-        <f t="shared" si="3"/>
-        <v>2839177.5882352944</v>
+        <f t="shared" si="6"/>
+        <v>2227056.0588235296</v>
       </c>
       <c r="J54" s="10">
-        <f t="shared" ref="J54:J56" si="5">K54/F54</f>
-        <v>14269.74912037552</v>
+        <f t="shared" si="2"/>
+        <v>16563.079001867944</v>
       </c>
       <c r="K54" s="21">
-        <v>2413300.9500000002</v>
+        <v>1892997.65</v>
       </c>
       <c r="L54" s="10">
-        <f t="shared" ref="L54:L56" si="6">M54/F54</f>
-        <v>13430.352109816393</v>
+        <f t="shared" si="3"/>
+        <v>15588.780262786466</v>
       </c>
       <c r="M54" s="21">
-        <v>2271342.0699999998</v>
+        <v>1781644.85</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -3053,88 +3066,358 @@
         <v>4</v>
       </c>
       <c r="B55" s="8">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C55" s="8">
         <v>2</v>
       </c>
       <c r="D55" s="8">
-        <v>112.4</v>
+        <v>96.69</v>
       </c>
       <c r="E55" s="9">
-        <v>56.720068589999997</v>
+        <v>20.199899290000001</v>
       </c>
       <c r="F55" s="9">
-        <v>169.12006859000002</v>
+        <v>116.88989929</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H55" s="10">
-        <f t="shared" si="4"/>
-        <v>16787.940141618259</v>
+        <f t="shared" si="0"/>
+        <v>19560.972905524493</v>
       </c>
       <c r="I55" s="21">
-        <f t="shared" si="3"/>
-        <v>2839177.5882352944</v>
+        <f t="shared" si="6"/>
+        <v>2286480.1529411767</v>
       </c>
       <c r="J55" s="10">
-        <f t="shared" si="5"/>
-        <v>14269.74912037552</v>
+        <f t="shared" si="2"/>
+        <v>16626.826969695816</v>
       </c>
       <c r="K55" s="21">
-        <v>2413300.9500000002</v>
+        <v>1943508.13</v>
       </c>
       <c r="L55" s="10">
-        <f t="shared" si="6"/>
-        <v>13430.352109816393</v>
+        <f t="shared" si="3"/>
+        <v>15648.778304290043</v>
       </c>
       <c r="M55" s="21">
-        <v>2271342.0699999998</v>
+        <v>1829184.12</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B56" s="8">
-        <v>1012</v>
+        <v>528</v>
       </c>
       <c r="C56" s="8">
         <v>2</v>
       </c>
       <c r="D56" s="8">
+        <v>96.69</v>
+      </c>
+      <c r="E56" s="9">
+        <v>20.199899290000001</v>
+      </c>
+      <c r="F56" s="9">
+        <v>116.88989929</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="10">
+        <f t="shared" si="0"/>
+        <v>19620.929879980384</v>
+      </c>
+      <c r="I56" s="21">
+        <f t="shared" si="6"/>
+        <v>2293488.5176470587</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" si="2"/>
+        <v>16677.790397983325</v>
+      </c>
+      <c r="K56" s="21">
+        <v>1949465.24</v>
+      </c>
+      <c r="L56" s="10">
+        <f t="shared" si="3"/>
+        <v>15696.743868757592</v>
+      </c>
+      <c r="M56" s="21">
+        <v>1834790.81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
+        <v>3</v>
+      </c>
+      <c r="B57" s="8">
+        <v>311</v>
+      </c>
+      <c r="C57" s="8">
+        <v>2</v>
+      </c>
+      <c r="D57" s="8">
+        <v>96.66</v>
+      </c>
+      <c r="E57" s="9">
+        <v>17.630202310000001</v>
+      </c>
+      <c r="F57" s="9">
+        <v>114.29020231</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="10">
+        <f t="shared" si="0"/>
+        <v>20818.285476211349</v>
+      </c>
+      <c r="I57" s="21">
+        <f t="shared" si="6"/>
+        <v>2379326.0588235296</v>
+      </c>
+      <c r="J57" s="10">
+        <f t="shared" si="2"/>
+        <v>17695.542654779645</v>
+      </c>
+      <c r="K57" s="21">
+        <v>2022427.15</v>
+      </c>
+      <c r="L57" s="10">
+        <f t="shared" si="3"/>
+        <v>16654.628406703363</v>
+      </c>
+      <c r="M57" s="21">
+        <v>1903460.85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="8">
+        <v>6</v>
+      </c>
+      <c r="B58" s="8">
+        <v>628</v>
+      </c>
+      <c r="C58" s="8">
+        <v>2</v>
+      </c>
+      <c r="D58" s="8">
+        <v>96.69</v>
+      </c>
+      <c r="E58" s="9">
+        <v>24.43999221</v>
+      </c>
+      <c r="F58" s="9">
+        <v>121.12999221</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="10">
+        <f t="shared" si="0"/>
+        <v>19680.871210968173</v>
+      </c>
+      <c r="I58" s="21">
+        <f t="shared" si="6"/>
+        <v>2383943.7764705881</v>
+      </c>
+      <c r="J58" s="10">
+        <f t="shared" si="2"/>
+        <v>16728.740529322949</v>
+      </c>
+      <c r="K58" s="21">
+        <v>2026352.21</v>
+      </c>
+      <c r="L58" s="10">
+        <f t="shared" si="3"/>
+        <v>15744.696959062077</v>
+      </c>
+      <c r="M58" s="21">
+        <v>1907155.02</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="8">
+        <v>8</v>
+      </c>
+      <c r="B59" s="8">
+        <v>828</v>
+      </c>
+      <c r="C59" s="8">
+        <v>2</v>
+      </c>
+      <c r="D59" s="8">
+        <v>96.69</v>
+      </c>
+      <c r="E59" s="9">
+        <v>24.43999221</v>
+      </c>
+      <c r="F59" s="9">
+        <v>121.12999221</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="10">
+        <f t="shared" si="0"/>
+        <v>19800.785069137175</v>
+      </c>
+      <c r="I59" s="21">
+        <f t="shared" si="6"/>
+        <v>2398468.9411764704</v>
+      </c>
+      <c r="J59" s="10">
+        <f t="shared" si="2"/>
+        <v>16830.667308766602</v>
+      </c>
+      <c r="K59" s="21">
+        <v>2038698.6</v>
+      </c>
+      <c r="L59" s="10">
+        <f t="shared" si="3"/>
+        <v>15840.62811358452</v>
+      </c>
+      <c r="M59" s="21">
+        <v>1918775.16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>3</v>
+      </c>
+      <c r="B60" s="8">
+        <v>326</v>
+      </c>
+      <c r="C60" s="8">
+        <v>2</v>
+      </c>
+      <c r="D60" s="8">
+        <v>112.4</v>
+      </c>
+      <c r="E60" s="9">
+        <v>56.720068589999997</v>
+      </c>
+      <c r="F60" s="9">
+        <v>169.12006859000002</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" s="10">
+        <f t="shared" si="0"/>
+        <v>16787.940141618259</v>
+      </c>
+      <c r="I60" s="21">
+        <f t="shared" si="6"/>
+        <v>2839177.5882352944</v>
+      </c>
+      <c r="J60" s="10">
+        <f t="shared" si="2"/>
+        <v>14269.74912037552</v>
+      </c>
+      <c r="K60" s="21">
+        <v>2413300.9500000002</v>
+      </c>
+      <c r="L60" s="10">
+        <f t="shared" si="3"/>
+        <v>13430.352109816393</v>
+      </c>
+      <c r="M60" s="21">
+        <v>2271342.0699999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="8">
+        <v>4</v>
+      </c>
+      <c r="B61" s="8">
+        <v>426</v>
+      </c>
+      <c r="C61" s="8">
+        <v>2</v>
+      </c>
+      <c r="D61" s="8">
+        <v>112.4</v>
+      </c>
+      <c r="E61" s="9">
+        <v>56.720068589999997</v>
+      </c>
+      <c r="F61" s="9">
+        <v>169.12006859000002</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" s="10">
+        <f t="shared" si="0"/>
+        <v>16787.940141618259</v>
+      </c>
+      <c r="I61" s="21">
+        <f t="shared" si="6"/>
+        <v>2839177.5882352944</v>
+      </c>
+      <c r="J61" s="10">
+        <f t="shared" si="2"/>
+        <v>14269.74912037552</v>
+      </c>
+      <c r="K61" s="21">
+        <v>2413300.9500000002</v>
+      </c>
+      <c r="L61" s="10">
+        <f t="shared" si="3"/>
+        <v>13430.352109816393</v>
+      </c>
+      <c r="M61" s="21">
+        <v>2271342.0699999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="8">
+        <v>10</v>
+      </c>
+      <c r="B62" s="8">
+        <v>1012</v>
+      </c>
+      <c r="C62" s="8">
+        <v>2</v>
+      </c>
+      <c r="D62" s="8">
         <v>108.11</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E62" s="9">
         <v>134.47987959</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F62" s="9">
         <v>242.58987959000001</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G62" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H56" s="10">
-        <f t="shared" si="4"/>
+      <c r="H62" s="10">
+        <f t="shared" si="0"/>
         <v>13490.321169895156</v>
       </c>
-      <c r="I56" s="21">
-        <f t="shared" si="3"/>
+      <c r="I62" s="21">
+        <f t="shared" si="6"/>
         <v>3272615.3882352943</v>
       </c>
-      <c r="J56" s="10">
-        <f t="shared" si="5"/>
+      <c r="J62" s="10">
+        <f t="shared" si="2"/>
         <v>11466.772994410883</v>
       </c>
-      <c r="K56" s="21">
+      <c r="K62" s="21">
         <v>2781723.08</v>
       </c>
-      <c r="L56" s="10">
-        <f t="shared" si="6"/>
+      <c r="L62" s="10">
+        <f t="shared" si="3"/>
         <v>10792.256933491311</v>
       </c>
-      <c r="M56" s="21">
+      <c r="M62" s="21">
         <v>2618092.31</v>
       </c>
     </row>

</xml_diff>